<commit_message>
New files and scripts added in Jackhmmer analysis
</commit_message>
<xml_diff>
--- a/Data/03_Homologs_Jackhmmer/Homologs_renamed.xlsx
+++ b/Data/03_Homologs_Jackhmmer/Homologs_renamed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/147a029199edd8ae/PG Materials/Semester3/FliF/Data/03_Homologs_Jackhmmer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="8_{8811EEEA-E01A-A54D-97D7-E49CF846C6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56D55020-3CE1-0145-B9B2-D984CC5D23B5}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="8_{8811EEEA-E01A-A54D-97D7-E49CF846C6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05586E0A-E020-F14C-AABE-D999A1F82742}"/>
   <bookViews>
-    <workbookView xWindow="32960" yWindow="1620" windowWidth="29340" windowHeight="18880" xr2:uid="{629EC489-E702-E64A-8AA6-5C662C675032}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29340" windowHeight="18880" xr2:uid="{629EC489-E702-E64A-8AA6-5C662C675032}"/>
   </bookViews>
   <sheets>
     <sheet name="protein" sheetId="3" r:id="rId1"/>
@@ -6562,8 +6562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B8448D-5FB7-4148-A42C-2E5B234EE183}">
   <dimension ref="A1:D1018"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A986" workbookViewId="0">
+      <selection activeCell="A1009" sqref="A1009"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21843,7 +21843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77BBB804-9063-B44C-B854-D40F785877DB}">
   <dimension ref="A1:Q1018"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="G984" workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
3D structures were obtained for the jackhmmer results
</commit_message>
<xml_diff>
--- a/Data/03_Homologs_Jackhmmer/Homologs_renamed.xlsx
+++ b/Data/03_Homologs_Jackhmmer/Homologs_renamed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/147a029199edd8ae/PG Materials/Semester3/FliF/Data/03_Homologs_Jackhmmer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="8_{8811EEEA-E01A-A54D-97D7-E49CF846C6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05586E0A-E020-F14C-AABE-D999A1F82742}"/>
+  <xr:revisionPtr revIDLastSave="82" documentId="8_{8811EEEA-E01A-A54D-97D7-E49CF846C6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA3A7B99-EBBC-4545-AB87-816B56BC0775}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29340" windowHeight="18880" xr2:uid="{629EC489-E702-E64A-8AA6-5C662C675032}"/>
+    <workbookView xWindow="160" yWindow="920" windowWidth="15320" windowHeight="18580" xr2:uid="{629EC489-E702-E64A-8AA6-5C662C675032}"/>
   </bookViews>
   <sheets>
     <sheet name="protein" sheetId="3" r:id="rId1"/>
@@ -6562,8 +6562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B8448D-5FB7-4148-A42C-2E5B234EE183}">
   <dimension ref="A1:D1018"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A986" workbookViewId="0">
-      <selection activeCell="A1009" sqref="A1009"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21482,7 +21482,7 @@
         <v>10</v>
       </c>
       <c r="D995" t="str">
-        <f t="shared" si="15"/>
+        <f>A995&amp;"_"&amp;B995&amp;"_"&amp;C995</f>
         <v>AEM21723.1_Brachyspira_FliF</v>
       </c>
     </row>

</xml_diff>